<commit_message>
Entrega Flujo de proyectos Minigranjas
</commit_message>
<xml_diff>
--- a/data/Flujo_proyectos_Minigranjas/SEGUIMIENTO NUEVOS NEGOCIOS.xlsx
+++ b/data/Flujo_proyectos_Minigranjas/SEGUIMIENTO NUEVOS NEGOCIOS.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMOSCOSO\Documents\dev\cash_flow_investment_automatization\data\Flujo_proyectos_Minigranjas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7213AF3A-2F9C-4385-9E89-97DA2D5ACA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35FABB5-5BAB-4904-85D4-0BFC50E514CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9772" xr2:uid="{62E5C20F-0C35-425C-890E-5C014F72F002}"/>
   </bookViews>
   <sheets>
     <sheet name="BD" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BD!$A$1:$E$23</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -153,6 +156,36 @@
   </si>
   <si>
     <t>Evolti 3</t>
+  </si>
+  <si>
+    <t>Predio</t>
+  </si>
+  <si>
+    <t>CAU044_ElPrado</t>
+  </si>
+  <si>
+    <t>CAU044_ElPrado_2</t>
+  </si>
+  <si>
+    <t>CAU044_ElPrado_3</t>
+  </si>
+  <si>
+    <t>CAU062_Beer-Sebas_1</t>
+  </si>
+  <si>
+    <t>CAU062_Beer-Sebas_2</t>
+  </si>
+  <si>
+    <t>CAU062_Beer-Sebas_3</t>
+  </si>
+  <si>
+    <t>CAU059_Predio-Estrecho_3</t>
+  </si>
+  <si>
+    <t>NAR031_Chachagui1</t>
+  </si>
+  <si>
+    <t>VAL002 - Andalucia</t>
   </si>
 </sst>
 </file>
@@ -214,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,7 +262,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9CE56D-DA9C-4CCD-BA7D-BB43CE25554D}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -584,9 +616,10 @@
     <col min="2" max="2" width="17.4609375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.765625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="17.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +632,11 @@
       <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -610,7 +646,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -620,7 +656,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -630,7 +666,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -641,8 +677,11 @@
       <c r="D5" s="5">
         <v>46045</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -654,7 +693,7 @@
         <v>45854</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -668,7 +707,7 @@
         <v>45902</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -682,7 +721,7 @@
         <v>45988</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -696,7 +735,7 @@
         <v>45981</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -710,7 +749,7 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -722,12 +761,12 @@
         <v>45976</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>26</v>
@@ -736,7 +775,7 @@
         <v>46052</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -750,7 +789,7 @@
         <v>46096</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -764,7 +803,7 @@
         <v>46096</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -773,8 +812,11 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -785,8 +827,11 @@
         <v>21</v>
       </c>
       <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -797,8 +842,11 @@
         <v>28</v>
       </c>
       <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -811,8 +859,11 @@
       <c r="D18" s="5">
         <v>46188</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -825,8 +876,11 @@
       <c r="D19" s="5">
         <v>46157</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -839,32 +893,38 @@
       <c r="D20" s="5">
         <v>46203</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="6" t="s">
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="5">
         <v>46203</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -872,6 +932,9 @@
         <v>36</v>
       </c>
       <c r="D23" s="5"/>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>